<commit_message>
add regexp columns Variables.csv
</commit_message>
<xml_diff>
--- a/dictionaries/methyl/2_0/lifecycle_2_0_methyl.xlsx
+++ b/dictionaries/methyl/2_0/lifecycle_2_0_methyl.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="127">
   <si>
     <t>table</t>
   </si>
@@ -396,12 +396,6 @@
   </si>
   <si>
     <t>Difference between Lee refined RPC clock and chronological GA from methylclock</t>
-  </si>
-  <si>
-    <t>variable</t>
-  </si>
-  <si>
-    <t>missing</t>
   </si>
 </sst>
 </file>
@@ -1992,30 +1986,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>